<commit_message>
Added setup of kaggle data, data combiner, final network setup, qk calculator, stats.
</commit_message>
<xml_diff>
--- a/code/python/kaggle_data_stats.xlsx
+++ b/code/python/kaggle_data_stats.xlsx
@@ -1,21 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="training" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,17 +66,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +377,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>25810</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2/SUM(B2:B6)</f>
+        <v>0.73478335136366224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2443</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3/SUM(B2:B6)</f>
+        <v>6.9549621363092867E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5292</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4/SUM(B2:B6)</f>
+        <v>0.1506576325229175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>873</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5/SUM(B2:B6)</f>
+        <v>2.4853384957011899E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>708</v>
+      </c>
+      <c r="C6" s="1">
+        <f>B6/SUM(B2:B6)</f>
+        <v>2.0156009793315492E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>39533</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2/SUM(B2:B6)</f>
+        <v>0.73788636703001342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3762</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3/SUM(B2:B6)</f>
+        <v>7.0218008063311937E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7861</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4/SUM(B2:B6)</f>
+        <v>0.1467261460355383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1214</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5/SUM(B2:B6)</f>
+        <v>2.2659399731222937E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1206</v>
+      </c>
+      <c r="C6" s="1">
+        <f>B6/SUM(B2:B6)</f>
+        <v>2.2510079139913396E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Different Color Normalization and Networks.
Disc and Vessel networks altered with different color normalization.
Different color normalization for Kaggle network.
</commit_message>
<xml_diff>
--- a/code/python/kaggle_data_stats.xlsx
+++ b/code/python/kaggle_data_stats.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -72,7 +72,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Pretraining tested and more network structions.
</commit_message>
<xml_diff>
--- a/code/python/kaggle_data_stats.xlsx
+++ b/code/python/kaggle_data_stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="training" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Class</t>
   </si>
@@ -24,6 +24,24 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Mild Non-Proliferative DR</t>
+  </si>
+  <si>
+    <t>Proliferative DR</t>
+  </si>
+  <si>
+    <t>Moderate Non-Proliferative DR</t>
+  </si>
+  <si>
+    <t>Severe Non-Proliferative DR</t>
   </si>
 </sst>
 </file>
@@ -378,86 +396,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>25810</v>
       </c>
-      <c r="C2" s="1">
-        <f>B2/SUM(B2:B6)</f>
+      <c r="D2" s="1">
+        <f>C2/SUM(C2:C6)</f>
         <v>0.73478335136366224</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>2443</v>
       </c>
-      <c r="C3" s="1">
-        <f>B3/SUM(B2:B6)</f>
+      <c r="D3" s="1">
+        <f>C3/SUM(C2:C6)</f>
         <v>6.9549621363092867E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>5292</v>
       </c>
-      <c r="C4" s="1">
-        <f>B4/SUM(B2:B6)</f>
+      <c r="D4" s="1">
+        <f>C4/SUM(C2:C6)</f>
         <v>0.1506576325229175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>873</v>
       </c>
-      <c r="C5" s="1">
-        <f>B5/SUM(B2:B6)</f>
+      <c r="D5" s="1">
+        <f>C5/SUM(C2:C6)</f>
         <v>2.4853384957011899E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>708</v>
       </c>
-      <c r="C6" s="1">
-        <f>B6/SUM(B2:B6)</f>
+      <c r="D6" s="1">
+        <f>C6/SUM(C2:C6)</f>
         <v>2.0156009793315492E-2</v>
       </c>
     </row>
@@ -468,82 +505,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>39533</v>
       </c>
-      <c r="C2" s="1">
-        <f>B2/SUM(B2:B6)</f>
+      <c r="D2" s="1">
+        <f>C2/SUM(C2:C6)</f>
         <v>0.73788636703001342</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>3762</v>
       </c>
-      <c r="C3" s="1">
-        <f>B3/SUM(B2:B6)</f>
+      <c r="D3" s="1">
+        <f>C3/SUM(C2:C6)</f>
         <v>7.0218008063311937E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>7861</v>
       </c>
-      <c r="C4" s="1">
-        <f>B4/SUM(B2:B6)</f>
+      <c r="D4" s="1">
+        <f>C4/SUM(C2:C6)</f>
         <v>0.1467261460355383</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>1214</v>
       </c>
-      <c r="C5" s="1">
-        <f>B5/SUM(B2:B6)</f>
+      <c r="D5" s="1">
+        <f>C5/SUM(C2:C6)</f>
         <v>2.2659399731222937E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>1206</v>
       </c>
-      <c r="C6" s="1">
-        <f>B6/SUM(B2:B6)</f>
+      <c r="D6" s="1">
+        <f>C6/SUM(C2:C6)</f>
         <v>2.2510079139913396E-2</v>
       </c>
     </row>

</xml_diff>